<commit_message>
updated license cleaned up code removed unused sections of code added in duration option for load dump calculations removed non UnitConversion.py unit conversions debug mode now demo mode. Auto runs ASCR Drake 795 26 with default config
</commit_message>
<xml_diff>
--- a/Sample/config-sample.xlsx
+++ b/Sample/config-sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8784a4c37ac16e51/Documents/Projects/Python/IEEE738-2012/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8784a4c37ac16e51/Documents/Projects/Python/IEEE738-2012/Sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{20139EA1-6448-4729-8D64-16A5AB5F184D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A7D272E-1B6D-4C32-ACDA-BD680A53508F}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{20139EA1-6448-4729-8D64-16A5AB5F184D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03340C9B-ABA0-42CA-BDE6-07B668C4ED98}"/>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="3040" windowWidth="19200" windowHeight="11170" xr2:uid="{7BCA82A4-9B05-41C2-838F-B9D27C2E09DE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{7BCA82A4-9B05-41C2-838F-B9D27C2E09DE}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
-  <si>
-    <t>threshold</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>solar absorptivity</t>
   </si>
@@ -149,6 +146,15 @@
   </si>
   <si>
     <t>m</t>
+  </si>
+  <si>
+    <t>design summer temperature</t>
+  </si>
+  <si>
+    <t>design winter temperature</t>
+  </si>
+  <si>
+    <t>duration (minutes)</t>
   </si>
 </sst>
 </file>
@@ -201,6 +207,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -503,45 +513,44 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA3"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:AA3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.08984375" customWidth="1"/>
-    <col min="16" max="16" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.08984375" customWidth="1"/>
+    <col min="15" max="15" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -550,43 +559,43 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>22</v>
       </c>
       <c r="G1" t="s">
         <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
         <v>19</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
       </c>
       <c r="K1" t="s">
         <v>20</v>
       </c>
       <c r="L1" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="M1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N1" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="O1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="P1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="Q1" t="s">
         <v>10</v>
@@ -598,194 +607,212 @@
         <v>12</v>
       </c>
       <c r="T1" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="U1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="V1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="W1" t="s">
         <v>29</v>
       </c>
       <c r="X1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y1" t="s">
         <v>30</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>34</v>
       </c>
       <c r="Z1" t="s">
         <v>31</v>
       </c>
       <c r="AA1" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>0.9</v>
+      </c>
+      <c r="C2">
+        <v>0.7</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>2.5329999999999999</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>90</v>
+      </c>
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="B2">
-        <v>1E-4</v>
-      </c>
-      <c r="C2">
-        <v>0.9</v>
-      </c>
-      <c r="D2">
-        <v>0.7</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>2.5329999999999999</v>
-      </c>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2">
+      <c r="J2">
         <v>90</v>
       </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2">
-        <v>90</v>
-      </c>
-      <c r="L2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2">
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2">
         <v>200</v>
       </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
       <c r="N2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="O2">
+        <v>40</v>
       </c>
       <c r="P2">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="Q2">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="R2">
-        <v>6</v>
+        <v>2009</v>
       </c>
       <c r="S2">
-        <v>2009</v>
-      </c>
-      <c r="T2">
         <v>1400</v>
+      </c>
+      <c r="T2" t="s">
+        <v>13</v>
       </c>
       <c r="U2" t="s">
         <v>14</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2">
+        <v>-15</v>
+      </c>
+      <c r="W2">
+        <v>40</v>
+      </c>
+      <c r="X2">
+        <v>5</v>
+      </c>
+      <c r="Y2">
+        <v>35</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA2">
+        <v>35</v>
+      </c>
+      <c r="AB2">
+        <v>10</v>
+      </c>
+      <c r="AC2">
         <v>15</v>
       </c>
-      <c r="W2">
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3">
+        <v>0.9</v>
+      </c>
+      <c r="C3">
+        <v>0.7</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>0.77205000000000001</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3">
+        <v>90</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3">
+        <v>90</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3">
+        <v>60.96</v>
+      </c>
+      <c r="M3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3">
+        <v>40</v>
+      </c>
+      <c r="P3">
+        <v>10</v>
+      </c>
+      <c r="Q3">
+        <v>6</v>
+      </c>
+      <c r="R3">
+        <v>2009</v>
+      </c>
+      <c r="S3">
+        <v>1400</v>
+      </c>
+      <c r="T3" t="s">
+        <v>34</v>
+      </c>
+      <c r="U3" t="s">
+        <v>14</v>
+      </c>
+      <c r="V3">
         <v>-15</v>
       </c>
-      <c r="X2">
+      <c r="W3">
         <v>40</v>
       </c>
-      <c r="Y2">
+      <c r="X3">
         <v>5</v>
       </c>
-      <c r="Z2">
+      <c r="Y3">
         <v>35</v>
       </c>
-      <c r="AA2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3">
-        <v>1E-4</v>
-      </c>
-      <c r="C3">
-        <v>0.9</v>
-      </c>
-      <c r="D3">
-        <v>0.7</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>0.77205000000000001</v>
-      </c>
-      <c r="H3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3">
-        <v>90</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3">
-        <v>90</v>
-      </c>
-      <c r="L3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3">
-        <v>60.96</v>
-      </c>
-      <c r="N3" t="s">
-        <v>37</v>
-      </c>
-      <c r="O3" t="s">
-        <v>28</v>
-      </c>
-      <c r="P3">
+      <c r="Z3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA3">
         <v>40</v>
       </c>
-      <c r="Q3">
-        <v>10</v>
-      </c>
-      <c r="R3">
-        <v>6</v>
-      </c>
-      <c r="S3">
-        <v>2009</v>
-      </c>
-      <c r="T3">
-        <v>1400</v>
-      </c>
-      <c r="U3" t="s">
-        <v>35</v>
-      </c>
-      <c r="V3" t="s">
+      <c r="AB3">
+        <v>5</v>
+      </c>
+      <c r="AC3">
         <v>15</v>
-      </c>
-      <c r="W3">
-        <v>-15</v>
-      </c>
-      <c r="X3">
-        <v>40</v>
-      </c>
-      <c r="Y3">
-        <v>5</v>
-      </c>
-      <c r="Z3">
-        <v>35</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>